<commit_message>
test: update grid6 data
</commit_message>
<xml_diff>
--- a/tests/test_data/grid6.xlsx
+++ b/tests/test_data/grid6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Work\YDev\EOS\vstu-xls\tests\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635BAC7F-738A-45A3-B6D8-97A095FF8420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20272AAC-DD20-4951-8531-743DF7C9CC86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-3960" windowWidth="19440" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="13">
   <si>
     <t>.</t>
   </si>
   <si>
     <t>*</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>A</t>
@@ -59,6 +56,9 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
   <dimension ref="A1:AN37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB24" sqref="AB24"/>
+      <selection activeCell="A20" sqref="A20:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,7 +548,7 @@
         <v>0</v>
       </c>
       <c r="AH1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AI1" s="4">
         <v>8</v>
@@ -663,7 +663,7 @@
         <v>31</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:40" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -884,22 +884,22 @@
       </c>
       <c r="AG7" s="7"/>
       <c r="AI7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AJ7" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="AK7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AL7" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="AM7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AN7" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="AN7" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:40" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -907,61 +907,61 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Y8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Z8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AF8" t="s">
         <v>0</v>
@@ -1034,34 +1034,34 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="X10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AF10" t="s">
         <v>0</v>
@@ -1099,37 +1099,37 @@
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="X11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Y11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AF11" t="s">
         <v>0</v>
@@ -1167,19 +1167,19 @@
         <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Y12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AF12" t="s">
         <v>0</v>
@@ -1217,25 +1217,25 @@
         <v>12</v>
       </c>
       <c r="J13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AA13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AB13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AF13" t="s">
         <v>0</v>
@@ -1273,37 +1273,37 @@
         <v>13</v>
       </c>
       <c r="L14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Z14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AA14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AF14" t="s">
         <v>0</v>
@@ -1341,16 +1341,16 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AF15" t="s">
         <v>0</v>
@@ -1388,55 +1388,55 @@
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="W16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="X16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Y16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Z16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AA16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AB16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AC16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AD16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AF16" t="s">
         <v>0</v>
@@ -1474,22 +1474,22 @@
         <v>16</v>
       </c>
       <c r="H17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AD17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AF17" t="s">
         <v>0</v>
@@ -1527,43 +1527,43 @@
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Y18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Z18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AA18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AB18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AD18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AF18" t="s">
         <v>0</v>
@@ -1601,34 +1601,34 @@
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AB19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AD19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AF19" t="s">
         <v>0</v>
@@ -1666,28 +1666,28 @@
         <v>19</v>
       </c>
       <c r="H20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AD20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AF20" t="s">
         <v>0</v>
@@ -1725,52 +1725,52 @@
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Y21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Z21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AA21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AB21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AC21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AD21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AF21" t="s">
         <v>0</v>
@@ -1804,8 +1804,8 @@
       </c>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>2</v>
+      <c r="A22">
+        <v>21</v>
       </c>
       <c r="AF22" t="s">
         <v>0</v>
@@ -1839,6 +1839,27 @@
       </c>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="K23" t="s">
+        <v>2</v>
+      </c>
+      <c r="L23" t="s">
+        <v>3</v>
+      </c>
+      <c r="M23" t="s">
+        <v>6</v>
+      </c>
+      <c r="N23" t="s">
+        <v>7</v>
+      </c>
+      <c r="O23" t="s">
+        <v>4</v>
+      </c>
+      <c r="P23" t="s">
+        <v>12</v>
+      </c>
       <c r="AH23">
         <v>16</v>
       </c>
@@ -1868,6 +1889,27 @@
       </c>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="K24" t="s">
+        <v>2</v>
+      </c>
+      <c r="L24" t="s">
+        <v>3</v>
+      </c>
+      <c r="M24" t="s">
+        <v>6</v>
+      </c>
+      <c r="N24" t="s">
+        <v>7</v>
+      </c>
+      <c r="O24" t="s">
+        <v>4</v>
+      </c>
+      <c r="P24" t="s">
+        <v>12</v>
+      </c>
       <c r="AH24">
         <v>17</v>
       </c>
@@ -1897,6 +1939,27 @@
       </c>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="K25" t="s">
+        <v>2</v>
+      </c>
+      <c r="L25" t="s">
+        <v>3</v>
+      </c>
+      <c r="M25" t="s">
+        <v>6</v>
+      </c>
+      <c r="N25" t="s">
+        <v>7</v>
+      </c>
+      <c r="O25" t="s">
+        <v>4</v>
+      </c>
+      <c r="P25" t="s">
+        <v>12</v>
+      </c>
       <c r="AH25">
         <v>18</v>
       </c>
@@ -1926,6 +1989,27 @@
       </c>
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="K26" t="s">
+        <v>2</v>
+      </c>
+      <c r="L26" t="s">
+        <v>3</v>
+      </c>
+      <c r="M26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N26" t="s">
+        <v>7</v>
+      </c>
+      <c r="O26" t="s">
+        <v>4</v>
+      </c>
+      <c r="P26" t="s">
+        <v>12</v>
+      </c>
       <c r="AH26">
         <v>19</v>
       </c>
@@ -1955,6 +2039,27 @@
       </c>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="K27" t="s">
+        <v>2</v>
+      </c>
+      <c r="L27" t="s">
+        <v>3</v>
+      </c>
+      <c r="M27" t="s">
+        <v>6</v>
+      </c>
+      <c r="N27" t="s">
+        <v>7</v>
+      </c>
+      <c r="O27" t="s">
+        <v>4</v>
+      </c>
+      <c r="P27" t="s">
+        <v>12</v>
+      </c>
       <c r="AH27">
         <v>20</v>
       </c>
@@ -1984,6 +2089,27 @@
       </c>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="K28" t="s">
+        <v>2</v>
+      </c>
+      <c r="L28" t="s">
+        <v>3</v>
+      </c>
+      <c r="M28" t="s">
+        <v>6</v>
+      </c>
+      <c r="N28" t="s">
+        <v>7</v>
+      </c>
+      <c r="O28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P28" t="s">
+        <v>12</v>
+      </c>
       <c r="AH28">
         <v>21</v>
       </c>

</xml_diff>